<commit_message>
updated the functionality of word suggestor!! also added the functionality to time traversar
</commit_message>
<xml_diff>
--- a/venv/words_library.xlsx
+++ b/venv/words_library.xlsx
@@ -381,2213 +381,2253 @@
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="0" t="inlineStr">
         <is>
           <t>a</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="0" t="inlineStr">
         <is>
           <t>between</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="0" t="inlineStr">
         <is>
           <t>could</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="0" t="inlineStr">
         <is>
           <t>Did</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="0" t="inlineStr">
         <is>
           <t>early</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="0" t="inlineStr">
         <is>
           <t>furry</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="0" t="inlineStr">
         <is>
           <t>gone</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="0" t="inlineStr">
         <is>
           <t>head.</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="0" t="inlineStr">
         <is>
           <t>inner</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="0" t="inlineStr">
         <is>
           <t>Jen.</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="0" t="inlineStr">
         <is>
           <t>know</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="0" t="inlineStr">
         <is>
           <t>Lee</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="0" t="inlineStr">
         <is>
           <t>mind</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="0" t="inlineStr">
         <is>
           <t>natural</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="O1" s="0" t="inlineStr">
         <is>
           <t>oceans</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="P1" s="0" t="inlineStr">
         <is>
           <t>PB</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="Q1" s="0" t="inlineStr">
         <is>
           <t>questions</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="R1" s="0" t="inlineStr">
         <is>
           <t>remaining</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="S1" s="0" t="inlineStr">
         <is>
           <t>Steve</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="T1" s="0" t="inlineStr">
         <is>
           <t>thought…alone”.</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="U1" s="0" t="inlineStr">
         <is>
           <t>used</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="V1" s="0" t="inlineStr">
         <is>
           <t>VCR</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="W1" s="0" t="inlineStr">
         <is>
           <t>With</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
+      <c r="Y1" s="0" t="inlineStr">
         <is>
           <t>years</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="0" t="inlineStr">
         <is>
           <t>atmosphere</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="0" t="inlineStr">
         <is>
           <t>biodiversity</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="0" t="inlineStr">
         <is>
           <t>core</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="0" t="inlineStr">
         <is>
           <t>drive</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="0" t="inlineStr">
         <is>
           <t>ever-growing,</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="0" t="inlineStr">
         <is>
           <t>featured</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="0" t="inlineStr">
         <is>
           <t>gravitational</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="0" t="inlineStr">
         <is>
           <t>hold</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="0" t="inlineStr">
         <is>
           <t>indicates</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="0" t="inlineStr">
         <is>
           <t>Jobs</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K2" s="0" t="inlineStr">
         <is>
           <t>known</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" s="0" t="inlineStr">
         <is>
           <t>long</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" s="0" t="inlineStr">
         <is>
           <t>Microsoft.</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="N2" s="0" t="inlineStr">
         <is>
           <t>next?</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O2" s="0" t="inlineStr">
         <is>
           <t>orbits</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="P2" s="0" t="inlineStr">
         <is>
           <t>plates</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="R2" s="0" t="inlineStr">
         <is>
           <t>remains</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="S2" s="0" t="inlineStr">
         <is>
           <t>Solar</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="T2" s="0" t="inlineStr">
         <is>
           <t>To</t>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="U2" s="0" t="inlineStr">
         <is>
           <t>us</t>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
+      <c r="V2" s="0" t="inlineStr">
         <is>
           <t>voyaging</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="W2" s="0" t="inlineStr">
         <is>
           <t>world’s</t>
         </is>
       </c>
-      <c r="Y2" t="inlineStr">
+      <c r="Y2" s="0" t="inlineStr">
         <is>
           <t>You</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="0" t="inlineStr">
         <is>
           <t>astronomical</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="0" t="inlineStr">
         <is>
           <t>beginning</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="0" t="inlineStr">
         <is>
           <t>common</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="0" t="inlineStr">
         <is>
           <t>divided</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" s="0" t="inlineStr">
         <is>
           <t>Earth</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" s="0" t="inlineStr">
         <is>
           <t>first</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" s="0" t="inlineStr">
         <is>
           <t>grocery</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H3" s="0" t="inlineStr">
         <is>
           <t>has</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" s="0" t="inlineStr">
         <is>
           <t>Inc.</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" s="0" t="inlineStr">
         <is>
           <t>know!</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L3" s="0" t="inlineStr">
         <is>
           <t>life.</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M3" s="0" t="inlineStr">
         <is>
           <t>more</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
+      <c r="N3" s="0" t="inlineStr">
         <is>
           <t>named</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O3" s="0" t="inlineStr">
         <is>
           <t>objects</t>
         </is>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="P3" s="0" t="inlineStr">
         <is>
           <t>petabyte</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="R3" s="0" t="inlineStr">
         <is>
           <t>red</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="S3" s="0" t="inlineStr">
         <is>
           <t>space,</t>
         </is>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="T3" s="0" t="inlineStr">
         <is>
           <t>There</t>
         </is>
       </c>
-      <c r="V3" t="inlineStr">
+      <c r="V3" s="0" t="inlineStr">
         <is>
           <t>vary</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="W3" s="0" t="inlineStr">
         <is>
           <t>what</t>
         </is>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Y3" s="0" t="inlineStr">
         <is>
           <t>year.</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="0" t="inlineStr">
         <is>
           <t>ado,</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="0" t="inlineStr">
         <is>
           <t>brings</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="0" t="inlineStr">
         <is>
           <t>creature</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D4" s="0" t="inlineStr">
         <is>
           <t>distance</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E4" s="0" t="inlineStr">
         <is>
           <t>evidence,</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" s="0" t="inlineStr">
         <is>
           <t>from</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" s="0" t="inlineStr">
         <is>
           <t>generates</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H4" s="0" t="inlineStr">
         <is>
           <t>here</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" s="0" t="inlineStr">
         <is>
           <t>instead</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L4" s="0" t="inlineStr">
         <is>
           <t>look</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="M4" s="0" t="inlineStr">
         <is>
           <t>Moon</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="N4" s="0" t="inlineStr">
         <is>
           <t>now?</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="O4" s="0" t="inlineStr">
         <is>
           <t>object</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="P4" s="0" t="inlineStr">
         <is>
           <t>periods</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
+      <c r="R4" s="0" t="inlineStr">
         <is>
           <t>Recorder)</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="S4" s="0" t="inlineStr">
         <is>
           <t>strange</t>
         </is>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="T4" s="0" t="inlineStr">
         <is>
           <t>tidbits</t>
         </is>
       </c>
-      <c r="V4" t="inlineStr">
+      <c r="V4" s="0" t="inlineStr">
         <is>
           <t>View</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
+      <c r="W4" s="0" t="inlineStr">
         <is>
           <t>was</t>
         </is>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="Y4" s="0" t="inlineStr">
         <is>
           <t>you’ll</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="0" t="inlineStr">
         <is>
           <t>around</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="0" t="inlineStr">
         <is>
           <t>beneath</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>computers</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="0" t="inlineStr">
         <is>
           <t>described.</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="E5" s="0" t="inlineStr">
         <is>
           <t>example</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" s="0" t="inlineStr">
         <is>
           <t>founded</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" s="0" t="inlineStr">
         <is>
           <t>goats</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" s="0" t="inlineStr">
         <is>
           <t>history,</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" s="0" t="inlineStr">
         <is>
           <t>ice</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L5" s="0" t="inlineStr">
         <is>
           <t>lived</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr">
+      <c r="M5" s="0" t="inlineStr">
         <is>
           <t>migrate</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
+      <c r="N5" s="0" t="inlineStr">
         <is>
           <t>need?!</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="O5" s="0" t="inlineStr">
         <is>
           <t>occasionally</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="P5" s="0" t="inlineStr">
         <is>
           <t>Politically,</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="R5" s="0" t="inlineStr">
         <is>
           <t>refer</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
+      <c r="S5" s="0" t="inlineStr">
         <is>
           <t>states.</t>
         </is>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="T5" s="0" t="inlineStr">
         <is>
           <t>that</t>
         </is>
       </c>
-      <c r="V5" t="inlineStr">
+      <c r="V5" s="0" t="inlineStr">
         <is>
           <t>video.</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr">
+      <c r="W5" s="0" t="inlineStr">
         <is>
           <t>we’ve</t>
         </is>
       </c>
-      <c r="Y5" t="inlineStr">
+      <c r="Y5" s="0" t="inlineStr">
         <is>
           <t>your</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="0" t="inlineStr">
         <is>
           <t>and,</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="0" t="inlineStr">
         <is>
           <t>biosphere</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="0" t="inlineStr">
         <is>
           <t>Camera</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="D6" s="0" t="inlineStr">
         <is>
           <t>dating</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="E6" s="0" t="inlineStr">
         <is>
           <t>Earth's</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" s="0" t="inlineStr">
         <is>
           <t>Facebook?</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" s="0" t="inlineStr">
         <is>
           <t>gradually</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="H6" s="0" t="inlineStr">
         <is>
           <t>herded</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" s="0" t="inlineStr">
         <is>
           <t>islands.</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="L6" s="0" t="inlineStr">
         <is>
           <t>languages.Earth</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="M6" s="0" t="inlineStr">
         <is>
           <t>much</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="N6" s="0" t="inlineStr">
         <is>
           <t>Newton</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="O6" s="0" t="inlineStr">
         <is>
           <t>Or</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="P6" s="0" t="inlineStr">
         <is>
           <t>proliferation</t>
         </is>
       </c>
-      <c r="R6" t="inlineStr">
+      <c r="R6" s="0" t="inlineStr">
         <is>
           <t>recorded</t>
         </is>
       </c>
-      <c r="S6" t="inlineStr">
+      <c r="S6" s="0" t="inlineStr">
         <is>
           <t>Surprisingly,</t>
         </is>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="T6" s="0" t="inlineStr">
         <is>
           <t>terabytes</t>
         </is>
       </c>
-      <c r="W6" t="inlineStr">
+      <c r="W6" s="0" t="inlineStr">
         <is>
           <t>which</t>
         </is>
       </c>
-      <c r="Y6" t="inlineStr">
+      <c r="Y6" s="0" t="inlineStr">
         <is>
           <t>years.</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="0" t="inlineStr">
         <is>
           <t>affect</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="0" t="inlineStr">
         <is>
           <t>been</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" s="0" t="inlineStr">
         <is>
           <t>cute</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D7" s="0" t="inlineStr">
         <is>
           <t>didn’t</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="0" t="inlineStr">
         <is>
           <t>ever</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" s="0" t="inlineStr">
         <is>
           <t>Firefox,</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" s="0" t="inlineStr">
         <is>
           <t>gaming</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="H7" s="0" t="inlineStr">
         <is>
           <t>here!</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" s="0" t="inlineStr">
         <is>
           <t>Isaac</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L7" s="0" t="inlineStr">
         <is>
           <t>labor</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="M7" s="0" t="inlineStr">
         <is>
           <t>most</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
+      <c r="N7" s="0" t="inlineStr">
         <is>
           <t>number</t>
         </is>
       </c>
-      <c r="O7" t="inlineStr">
+      <c r="O7" s="0" t="inlineStr">
         <is>
           <t>orbital</t>
         </is>
       </c>
-      <c r="P7" t="inlineStr">
+      <c r="P7" s="0" t="inlineStr">
         <is>
           <t>period</t>
         </is>
       </c>
-      <c r="R7" t="inlineStr">
+      <c r="R7" s="0" t="inlineStr">
         <is>
           <t>rigid</t>
         </is>
       </c>
-      <c r="S7" t="inlineStr">
+      <c r="S7" s="0" t="inlineStr">
         <is>
           <t>solid</t>
         </is>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="T7" s="0" t="inlineStr">
         <is>
           <t>The</t>
         </is>
       </c>
-      <c r="W7" t="inlineStr">
+      <c r="W7" s="0" t="inlineStr">
         <is>
           <t>without</t>
         </is>
       </c>
-      <c r="Y7" t="inlineStr">
+      <c r="Y7" s="0" t="inlineStr">
         <is>
           <t>you</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="0" t="inlineStr">
         <is>
           <t>anaerobic</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="0" t="inlineStr">
         <is>
           <t>because</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C8" s="0" t="inlineStr">
         <is>
           <t>created</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="D8" s="0" t="inlineStr">
         <is>
           <t>densest</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="E8" s="0" t="inlineStr">
         <is>
           <t>Earth.</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" s="0" t="inlineStr">
         <is>
           <t>facts,</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" s="0" t="inlineStr">
         <is>
           <t>go</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="H8" s="0" t="inlineStr">
         <is>
           <t>how</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="I8" s="0" t="inlineStr">
         <is>
           <t>interior</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="L8" s="0" t="inlineStr">
         <is>
           <t>leading</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr">
+      <c r="M8" s="0" t="inlineStr">
         <is>
           <t>may</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr">
+      <c r="N8" s="0" t="inlineStr">
         <is>
           <t>not</t>
         </is>
       </c>
-      <c r="O8" t="inlineStr">
+      <c r="O8" s="0" t="inlineStr">
         <is>
           <t>Originally,</t>
         </is>
       </c>
-      <c r="P8" t="inlineStr">
+      <c r="P8" s="0" t="inlineStr">
         <is>
           <t>punctuated</t>
         </is>
       </c>
-      <c r="R8" t="inlineStr">
+      <c r="R8" s="0" t="inlineStr">
         <is>
           <t>rivers</t>
         </is>
       </c>
-      <c r="S8" t="inlineStr">
+      <c r="S8" s="0" t="inlineStr">
         <is>
           <t>seas</t>
         </is>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="T8" s="0" t="inlineStr">
         <is>
           <t>today</t>
         </is>
       </c>
-      <c r="W8" t="inlineStr">
+      <c r="W8" s="0" t="inlineStr">
         <is>
           <t>Within</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="0" t="inlineStr">
         <is>
           <t>ago.</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="0" t="inlineStr">
         <is>
           <t>border</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C9" s="0" t="inlineStr">
         <is>
           <t>collie</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D9" s="0" t="inlineStr">
         <is>
           <t>designed</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="E9" s="0" t="inlineStr">
         <is>
           <t>expansion,</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" s="0" t="inlineStr">
         <is>
           <t>four</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" s="0" t="inlineStr">
         <is>
           <t>give</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="H9" s="0" t="inlineStr">
         <is>
           <t>harbor</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I9" s="0" t="inlineStr">
         <is>
           <t>it</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="L9" s="0" t="inlineStr">
         <is>
           <t>lakes,</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="M9" s="0" t="inlineStr">
         <is>
           <t>Moon,</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="O9" s="0" t="inlineStr">
         <is>
           <t>on</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="P9" s="0" t="inlineStr">
         <is>
           <t>properties</t>
         </is>
       </c>
-      <c r="R9" t="inlineStr">
+      <c r="R9" s="0" t="inlineStr">
         <is>
           <t>rocky</t>
         </is>
       </c>
-      <c r="S9" t="inlineStr">
+      <c r="S9" s="0" t="inlineStr">
         <is>
           <t>sheet</t>
         </is>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="T9" s="0" t="inlineStr">
         <is>
           <t>top</t>
         </is>
       </c>
-      <c r="W9" t="inlineStr">
+      <c r="W9" s="0" t="inlineStr">
         <is>
           <t>world</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="0" t="inlineStr">
         <is>
           <t>an</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="0" t="inlineStr">
         <is>
           <t>began</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C10" s="0" t="inlineStr">
         <is>
           <t>currency</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="D10" s="0" t="inlineStr">
         <is>
           <t>Do</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="E10" s="0" t="inlineStr">
         <is>
           <t>equivalent</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" s="0" t="inlineStr">
         <is>
           <t>future</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G10" s="0" t="inlineStr">
         <is>
           <t>gadgets</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="H10" s="0" t="inlineStr">
         <is>
           <t>HD-TV</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" s="0" t="inlineStr">
         <is>
           <t>including</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="L10" s="0" t="inlineStr">
         <is>
           <t>logo</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="M10" s="0" t="inlineStr">
         <is>
           <t>mostly</t>
         </is>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="O10" s="0" t="inlineStr">
         <is>
           <t>organisms.</t>
         </is>
       </c>
-      <c r="P10" t="inlineStr">
+      <c r="P10" s="0" t="inlineStr">
         <is>
           <t>phrase</t>
         </is>
       </c>
-      <c r="R10" t="inlineStr">
+      <c r="R10" s="0" t="inlineStr">
         <is>
           <t>resources</t>
         </is>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="S10" s="0" t="inlineStr">
         <is>
           <t>species</t>
         </is>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="T10" s="0" t="inlineStr">
         <is>
           <t>this</t>
         </is>
       </c>
-      <c r="W10" t="inlineStr">
+      <c r="W10" s="0" t="inlineStr">
         <is>
           <t>widely;</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="0" t="inlineStr">
         <is>
           <t>axis</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B11" s="0" t="inlineStr">
         <is>
           <t>by</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C11" s="0" t="inlineStr">
         <is>
           <t>consisting</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="D11" s="0" t="inlineStr">
         <is>
           <t>days,</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="E11" s="0" t="inlineStr">
         <is>
           <t>eat</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" s="0" t="inlineStr">
         <is>
           <t>for</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="0" t="inlineStr">
         <is>
           <t>gravity</t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="H11" s="0" t="inlineStr">
         <is>
           <t>hard</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" s="0" t="inlineStr">
         <is>
           <t>inner-geek</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="L11" s="0" t="inlineStr">
         <is>
           <t>live</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="M11" s="0" t="inlineStr">
         <is>
           <t>must</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="O11" s="0" t="inlineStr">
         <is>
           <t>outer</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="P11" s="0" t="inlineStr">
         <is>
           <t>planets.</t>
         </is>
       </c>
-      <c r="R11" t="inlineStr">
+      <c r="R11" s="0" t="inlineStr">
         <is>
           <t>read</t>
         </is>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="S11" s="0" t="inlineStr">
         <is>
           <t>Sir</t>
         </is>
       </c>
-      <c r="T11" t="inlineStr">
+      <c r="T11" s="0" t="inlineStr">
         <is>
           <t>tech</t>
         </is>
       </c>
-      <c r="W11" t="inlineStr">
+      <c r="W11" s="0" t="inlineStr">
         <is>
           <t>we</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="0" t="inlineStr">
         <is>
           <t>axis,</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>bigger</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C12" s="0" t="inlineStr">
         <is>
           <t>Czech</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D12" s="0" t="inlineStr">
         <is>
           <t>drives</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
+      <c r="E12" s="0" t="inlineStr">
         <is>
           <t>earn</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" s="0" t="inlineStr">
         <is>
           <t>further</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" s="0" t="inlineStr">
         <is>
           <t>giants</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="H12" s="0" t="inlineStr">
         <is>
           <t>headquarters.</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" s="0" t="inlineStr">
         <is>
           <t>imagined.</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="L12" s="0" t="inlineStr">
         <is>
           <t>liquid</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="M12" s="0" t="inlineStr">
         <is>
           <t>millions</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="O12" s="0" t="inlineStr">
         <is>
           <t>orientation</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="P12" s="0" t="inlineStr">
         <is>
           <t>planet</t>
         </is>
       </c>
-      <c r="R12" t="inlineStr">
+      <c r="R12" s="0" t="inlineStr">
         <is>
           <t>rotation</t>
         </is>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="S12" s="0" t="inlineStr">
         <is>
           <t>size</t>
         </is>
       </c>
-      <c r="T12" t="inlineStr">
+      <c r="T12" s="0" t="inlineStr">
         <is>
           <t>than</t>
         </is>
       </c>
-      <c r="W12" t="inlineStr">
+      <c r="W12" s="0" t="inlineStr">
         <is>
           <t>work.</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="0" t="inlineStr">
         <is>
           <t>all</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B13" s="0" t="inlineStr">
         <is>
           <t>back</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C13" s="0" t="inlineStr">
         <is>
           <t>combination</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D13" s="0" t="inlineStr">
         <is>
           <t>depend</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="E13" s="0" t="inlineStr">
         <is>
           <t>extinct.</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" s="0" t="inlineStr">
         <is>
           <t>formed</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" s="0" t="inlineStr">
         <is>
           <t>Google,</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="H13" s="0" t="inlineStr">
         <is>
           <t>herder</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I13" s="0" t="inlineStr">
         <is>
           <t>If</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="L13" s="0" t="inlineStr">
         <is>
           <t>land</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr">
+      <c r="M13" s="0" t="inlineStr">
         <is>
           <t>magnetic</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="O13" s="0" t="inlineStr">
         <is>
           <t>of</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="P13" s="0" t="inlineStr">
         <is>
           <t>producing</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr">
+      <c r="R13" s="0" t="inlineStr">
         <is>
           <t>regions</t>
         </is>
       </c>
-      <c r="S13" t="inlineStr">
+      <c r="S13" s="0" t="inlineStr">
         <is>
           <t>several</t>
         </is>
       </c>
-      <c r="T13" t="inlineStr">
+      <c r="T13" s="0" t="inlineStr">
         <is>
           <t>these</t>
         </is>
       </c>
-      <c r="W13" t="inlineStr">
+      <c r="W13" s="0" t="inlineStr">
         <is>
           <t>works</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="0" t="inlineStr">
         <is>
           <t>appeared</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B14" s="0" t="inlineStr">
         <is>
           <t>bring</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="C14" s="0" t="inlineStr">
         <is>
           <t>convecting</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D14" s="0" t="inlineStr">
         <is>
           <t>did</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="E14" s="0" t="inlineStr">
         <is>
           <t>entire</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" s="0" t="inlineStr">
         <is>
           <t>find</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" s="0" t="inlineStr">
         <is>
           <t>grass</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="H14" s="0" t="inlineStr">
         <is>
           <t>history</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" s="0" t="inlineStr">
         <is>
           <t>internet,</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="L14" s="0" t="inlineStr">
         <is>
           <t>largest</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="M14" s="0" t="inlineStr">
         <is>
           <t>mowing</t>
         </is>
       </c>
-      <c r="O14" t="inlineStr">
+      <c r="O14" s="0" t="inlineStr">
         <is>
           <t>only</t>
         </is>
       </c>
-      <c r="P14" t="inlineStr">
+      <c r="P14" s="0" t="inlineStr">
         <is>
           <t>physical</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
+      <c r="R14" s="0" t="inlineStr">
         <is>
           <t>rotates</t>
         </is>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="S14" s="0" t="inlineStr">
         <is>
           <t>survival.</t>
         </is>
       </c>
-      <c r="T14" t="inlineStr">
+      <c r="T14" s="0" t="inlineStr">
         <is>
           <t>tectonics.</t>
         </is>
       </c>
-      <c r="W14" t="inlineStr">
+      <c r="W14" s="0" t="inlineStr">
         <is>
           <t>where</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="0" t="inlineStr">
         <is>
           <t>also</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="0" t="inlineStr">
         <is>
           <t>browser</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C15" s="0" t="inlineStr">
         <is>
           <t>covered</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D15" s="0" t="inlineStr">
         <is>
           <t>digital?</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" s="0" t="inlineStr">
         <is>
           <t>evolve</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" s="0" t="inlineStr">
         <is>
           <t>Find</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" s="0" t="inlineStr">
         <is>
           <t>geological</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H15" s="0" t="inlineStr">
         <is>
           <t>have</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I15" s="0" t="inlineStr">
         <is>
           <t>ice,</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="L15" s="0" t="inlineStr">
         <is>
           <t>layer</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="M15" s="0" t="inlineStr">
         <is>
           <t>meaning</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="O15" s="0" t="inlineStr">
         <is>
           <t>over</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="P15" s="0" t="inlineStr">
         <is>
           <t>polar</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr">
+      <c r="R15" s="0" t="inlineStr">
         <is>
           <t>right,</t>
         </is>
       </c>
-      <c r="S15" t="inlineStr">
+      <c r="S15" s="0" t="inlineStr">
         <is>
           <t>sitting</t>
         </is>
       </c>
-      <c r="T15" t="inlineStr">
+      <c r="T15" s="0" t="inlineStr">
         <is>
           <t>tectonic</t>
         </is>
       </c>
-      <c r="W15" t="inlineStr">
+      <c r="W15" s="0" t="inlineStr">
         <is>
           <t>Wozniak</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="0" t="inlineStr">
         <is>
           <t>at</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B16" s="0" t="inlineStr">
         <is>
           <t>Byung-Chull.</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="C16" s="0" t="inlineStr">
         <is>
           <t>core,</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="D16" s="0" t="inlineStr">
         <is>
           <t>During</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="E16" s="0" t="inlineStr">
         <is>
           <t>etymology</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" s="0" t="inlineStr">
         <is>
           <t>facts</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" s="0" t="inlineStr">
         <is>
           <t>Google</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="H16" s="0" t="inlineStr">
         <is>
           <t>humanoid</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="I16" s="0" t="inlineStr">
         <is>
           <t>is,</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="L16" s="0" t="inlineStr">
         <is>
           <t>life</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="M16" s="0" t="inlineStr">
         <is>
           <t>mantle</t>
         </is>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="O16" s="0" t="inlineStr">
         <is>
           <t>Over</t>
         </is>
       </c>
-      <c r="P16" t="inlineStr">
+      <c r="P16" s="0" t="inlineStr">
         <is>
           <t>panda!</t>
         </is>
       </c>
-      <c r="R16" t="inlineStr">
+      <c r="R16" s="0" t="inlineStr">
         <is>
           <t>respect</t>
         </is>
       </c>
-      <c r="S16" t="inlineStr">
+      <c r="S16" s="0" t="inlineStr">
         <is>
           <t>Since</t>
         </is>
       </c>
-      <c r="T16" t="inlineStr">
+      <c r="T16" s="0" t="inlineStr">
         <is>
           <t>translates</t>
         </is>
       </c>
-      <c r="W16" t="inlineStr">
+      <c r="W16" s="0" t="inlineStr">
         <is>
           <t>would</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="0" t="inlineStr">
         <is>
           <t>A</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B17" s="0" t="inlineStr">
         <is>
           <t>big</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="C17" s="0" t="inlineStr">
         <is>
           <t>Computer</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>df</t>
+        </is>
+      </c>
+      <c r="E17" s="0" t="inlineStr">
         <is>
           <t>Earth,</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" s="0" t="inlineStr">
         <is>
           <t>forever</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G17" s="0" t="inlineStr">
         <is>
           <t>get</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="H17" s="0" t="inlineStr">
         <is>
           <t>his</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I17" s="0" t="inlineStr">
         <is>
           <t>into</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="L17" s="0" t="inlineStr">
         <is>
           <t>lawn,</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr">
+      <c r="M17" s="0" t="inlineStr">
         <is>
           <t>majority</t>
         </is>
       </c>
-      <c r="O17" t="inlineStr">
+      <c r="O17" s="0" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="P17" t="inlineStr">
+      <c r="P17" s="0" t="inlineStr">
         <is>
           <t>pack.</t>
         </is>
       </c>
-      <c r="R17" t="inlineStr">
+      <c r="R17" s="0" t="inlineStr">
         <is>
           <t>rents</t>
         </is>
       </c>
-      <c r="S17" t="inlineStr">
+      <c r="S17" s="0" t="inlineStr">
         <is>
           <t>store</t>
         </is>
       </c>
-      <c r="T17" t="inlineStr">
+      <c r="T17" s="0" t="inlineStr">
         <is>
           <t>the</t>
         </is>
       </c>
-      <c r="W17" t="inlineStr">
+      <c r="W17" s="0" t="inlineStr">
         <is>
           <t>with</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="0" t="inlineStr">
         <is>
           <t>allowed</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="B18" s="0" t="inlineStr">
         <is>
           <t>bugs</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C18" s="0" t="inlineStr">
         <is>
           <t>continents</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="D18" s="0" t="inlineStr">
+        <is>
+          <t>d</t>
+        </is>
+      </c>
+      <c r="E18" s="0" t="inlineStr">
         <is>
           <t>evidence</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" s="0" t="inlineStr">
         <is>
           <t>fictional</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" s="0" t="inlineStr">
         <is>
           <t>GB</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="H18" s="0" t="inlineStr">
         <is>
           <t>hydrosphere.</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="I18" s="0" t="inlineStr">
         <is>
           <t>It</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="L18" s="0" t="inlineStr">
         <is>
           <t>later,</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="M18" s="0" t="inlineStr">
         <is>
           <t>MB,</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr">
+      <c r="O18" s="0" t="inlineStr">
         <is>
           <t>or</t>
         </is>
       </c>
-      <c r="P18" t="inlineStr">
+      <c r="P18" s="0" t="inlineStr">
         <is>
           <t>piano.</t>
         </is>
       </c>
-      <c r="R18" t="inlineStr">
+      <c r="R18" s="0" t="inlineStr">
         <is>
           <t>rotation.</t>
         </is>
       </c>
-      <c r="S18" t="inlineStr">
+      <c r="S18" s="0" t="inlineStr">
         <is>
           <t>sea</t>
         </is>
       </c>
-      <c r="T18" t="inlineStr">
+      <c r="T18" s="0" t="inlineStr">
         <is>
           <t>times.</t>
         </is>
       </c>
-      <c r="W18" t="inlineStr">
+      <c r="W18" s="0" t="inlineStr">
         <is>
           <t>word</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="0" t="inlineStr">
         <is>
           <t>Apple</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="B19" s="0" t="inlineStr">
         <is>
           <t>But</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="C19" s="0" t="inlineStr">
         <is>
           <t>comes</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="E19" s="0" t="inlineStr">
         <is>
           <t>Estimates</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" s="0" t="inlineStr">
         <is>
           <t>fox.</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" s="0" t="inlineStr">
         <is>
           <t>guessed!Samsung</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="H19" s="0" t="inlineStr">
         <is>
           <t>humans</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I19" s="0" t="inlineStr">
         <is>
           <t>I</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="M19" s="0" t="inlineStr">
         <is>
           <t>misbelief</t>
         </is>
       </c>
-      <c r="P19" t="inlineStr">
+      <c r="P19" s="0" t="inlineStr">
         <is>
           <t>plane,</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr">
+      <c r="R19" s="0" t="inlineStr">
         <is>
           <t>radiometric</t>
         </is>
       </c>
-      <c r="S19" t="inlineStr">
+      <c r="S19" s="0" t="inlineStr">
         <is>
           <t>sidereal</t>
         </is>
       </c>
-      <c r="T19" t="inlineStr">
+      <c r="T19" s="0" t="inlineStr">
         <is>
           <t>thrive.</t>
         </is>
       </c>
-      <c r="W19" t="inlineStr">
+      <c r="W19" s="0" t="inlineStr">
         <is>
           <t>written</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="0" t="inlineStr">
         <is>
           <t>Arctic</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B20" s="0" t="inlineStr">
         <is>
           <t>be</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="C20" s="0" t="inlineStr">
         <is>
           <t>constitute</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="E20" s="0" t="inlineStr">
         <is>
           <t>especially</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" s="0" t="inlineStr">
         <is>
           <t>Founders</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="I20" s="0" t="inlineStr">
         <is>
           <t>iron</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr">
+      <c r="M20" s="0" t="inlineStr">
         <is>
           <t>made</t>
         </is>
       </c>
-      <c r="P20" t="inlineStr">
+      <c r="P20" s="0" t="inlineStr">
         <is>
           <t>plate</t>
         </is>
       </c>
-      <c r="S20" t="inlineStr">
+      <c r="S20" s="0" t="inlineStr">
         <is>
           <t>surface</t>
         </is>
       </c>
-      <c r="T20" t="inlineStr">
+      <c r="T20" s="0" t="inlineStr">
         <is>
           <t>to</t>
         </is>
       </c>
-      <c r="W20" t="inlineStr">
+      <c r="W20" s="0" t="inlineStr">
         <is>
           <t>will</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="0" t="inlineStr">
         <is>
           <t>arisen</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B21" s="0" t="inlineStr">
         <is>
           <t>but</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="0" t="inlineStr">
         <is>
           <t>causes</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="E21" s="0" t="inlineStr">
         <is>
           <t>ever-changing</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" s="0" t="inlineStr">
         <is>
           <t>fall</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="I21" s="0" t="inlineStr">
         <is>
           <t>In</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="M21" s="0" t="inlineStr">
         <is>
           <t>March</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr">
+      <c r="P21" s="0" t="inlineStr">
         <is>
           <t>play</t>
         </is>
       </c>
-      <c r="S21" t="inlineStr">
+      <c r="S21" s="0" t="inlineStr">
         <is>
           <t>seasons</t>
         </is>
       </c>
-      <c r="T21" t="inlineStr">
+      <c r="T21" s="0" t="inlineStr">
         <is>
           <t>their</t>
         </is>
       </c>
-      <c r="W21" t="inlineStr">
+      <c r="W21" s="0" t="inlineStr">
         <is>
           <t>Way</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="0" t="inlineStr">
         <is>
           <t>apple</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B22" s="0" t="inlineStr">
         <is>
           <t>billion</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="E22" s="0" t="inlineStr">
         <is>
           <t>extinctions.</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" s="0" t="inlineStr">
         <is>
           <t>fresh</t>
         </is>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="I22" s="0" t="inlineStr">
         <is>
           <t>interacts</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="M22" s="0" t="inlineStr">
         <is>
           <t>mass</t>
         </is>
       </c>
-      <c r="S22" t="inlineStr">
+      <c r="S22" s="0" t="inlineStr">
         <is>
           <t>Sun,</t>
         </is>
       </c>
-      <c r="T22" t="inlineStr">
+      <c r="T22" s="0" t="inlineStr">
         <is>
           <t>tides,</t>
         </is>
       </c>
-      <c r="W22" t="inlineStr">
+      <c r="W22" s="0" t="inlineStr">
         <is>
           <t>water,</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="0" t="inlineStr">
         <is>
           <t>According</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="B23" s="0" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
         <is>
           <t>finding</t>
         </is>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="I23" s="0" t="inlineStr">
         <is>
           <t>in</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr">
+      <c r="M23" s="0" t="inlineStr">
         <is>
           <t>massive</t>
         </is>
       </c>
-      <c r="S23" t="inlineStr">
+      <c r="S23" s="0" t="inlineStr">
         <is>
           <t>surface,</t>
         </is>
       </c>
-      <c r="T23" t="inlineStr">
+      <c r="T23" s="0" t="inlineStr">
         <is>
           <t>technology</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="0" t="inlineStr">
         <is>
           <t>About</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>bf</t>
+        </is>
+      </c>
+      <c r="F24" s="0" t="inlineStr">
         <is>
           <t>field,</t>
         </is>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="I24" s="0" t="inlineStr">
         <is>
           <t>interesting</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr">
+      <c r="M24" s="0" t="inlineStr">
         <is>
           <t>Mountain</t>
         </is>
       </c>
-      <c r="S24" t="inlineStr">
+      <c r="S24" s="0" t="inlineStr">
         <is>
           <t>same</t>
         </is>
       </c>
-      <c r="T24" t="inlineStr">
+      <c r="T24" s="0" t="inlineStr">
         <is>
           <t>together</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="0" t="inlineStr">
         <is>
           <t>aerobic</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" s="0" t="inlineStr">
         <is>
           <t>forced</t>
         </is>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" s="0" t="inlineStr">
         <is>
           <t>is</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="M25" s="0" t="inlineStr">
         <is>
           <t>mankind,</t>
         </is>
       </c>
-      <c r="S25" t="inlineStr">
+      <c r="S25" s="0" t="inlineStr">
         <is>
           <t>So</t>
         </is>
       </c>
-      <c r="T25" t="inlineStr">
+      <c r="T25" s="0" t="inlineStr">
         <is>
           <t>time,</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="0" t="inlineStr">
         <is>
           <t>And</t>
         </is>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="I26" s="0" t="inlineStr">
         <is>
           <t>interaction</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr">
+      <c r="M26" s="0" t="inlineStr">
         <is>
           <t>money</t>
         </is>
       </c>
-      <c r="S26" t="inlineStr">
+      <c r="S26" s="0" t="inlineStr">
         <is>
           <t>sovereign</t>
         </is>
       </c>
-      <c r="T26" t="inlineStr">
+      <c r="T26" s="0" t="inlineStr">
         <is>
           <t>Technology,</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="0" t="inlineStr">
         <is>
           <t>and</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="I27" s="0" t="inlineStr">
         <is>
           <t>its</t>
         </is>
       </c>
-      <c r="M27" t="inlineStr">
+      <c r="M27" s="0" t="inlineStr">
         <is>
           <t>many</t>
         </is>
       </c>
-      <c r="S27" t="inlineStr">
+      <c r="S27" s="0" t="inlineStr">
         <is>
           <t>satellite.</t>
         </is>
       </c>
-      <c r="T27" t="inlineStr">
+      <c r="T27" s="0" t="inlineStr">
         <is>
           <t>through</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="0" t="inlineStr">
         <is>
           <t>April</t>
         </is>
       </c>
-      <c r="S28" t="inlineStr">
+      <c r="S28" s="0" t="inlineStr">
         <is>
           <t>slows</t>
         </is>
       </c>
-      <c r="T28" t="inlineStr">
+      <c r="T28" s="0" t="inlineStr">
         <is>
           <t>tilted</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="0" t="inlineStr">
         <is>
           <t>actually</t>
         </is>
       </c>
-      <c r="S29" t="inlineStr">
+      <c r="S29" s="0" t="inlineStr">
         <is>
           <t>Some</t>
         </is>
       </c>
-      <c r="T29" t="inlineStr">
+      <c r="T29" s="0" t="inlineStr">
         <is>
           <t>then,</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="0" t="inlineStr">
         <is>
           <t>across</t>
         </is>
       </c>
-      <c r="S30" t="inlineStr">
+      <c r="S30" s="0" t="inlineStr">
         <is>
           <t>Sun</t>
         </is>
       </c>
-      <c r="T30" t="inlineStr">
+      <c r="T30" s="0" t="inlineStr">
         <is>
           <t>third</t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="0" t="inlineStr">
         <is>
           <t>actual</t>
         </is>
       </c>
-      <c r="S31" t="inlineStr">
+      <c r="S31" s="0" t="inlineStr">
         <is>
           <t>surprising</t>
         </is>
       </c>
-      <c r="T31" t="inlineStr">
+      <c r="T31" s="0" t="inlineStr">
         <is>
           <t>tree,</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="0" t="inlineStr">
         <is>
           <t>active</t>
         </is>
       </c>
-      <c r="S32" t="inlineStr">
+      <c r="S32" s="0" t="inlineStr">
         <is>
           <t>such</t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="0" t="inlineStr">
         <is>
           <t>answers</t>
         </is>
       </c>
-      <c r="S33" t="inlineStr">
+      <c r="S33" s="0" t="inlineStr">
         <is>
           <t>System</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="0" t="inlineStr">
         <is>
           <t>Antarctic</t>
         </is>
       </c>
-      <c r="S34" t="inlineStr">
+      <c r="S34" s="0" t="inlineStr">
         <is>
           <t>stabilizes</t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="0" t="inlineStr">
         <is>
           <t>about</t>
         </is>
       </c>
+      <c r="S35" s="0" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="0" t="inlineStr">
         <is>
           <t>are</t>
         </is>
       </c>
+      <c r="S36" s="0" t="inlineStr">
+        <is>
+          <t>sddx</t>
+        </is>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="0" t="inlineStr">
         <is>
           <t>always</t>
         </is>
       </c>
+      <c r="S37" s="0" t="inlineStr">
+        <is>
+          <t>sdfhv</t>
+        </is>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="0" t="inlineStr">
         <is>
           <t>as</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>sdfgea</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding the functionality of mic !!
</commit_message>
<xml_diff>
--- a/venv/words_library.xlsx
+++ b/venv/words_library.xlsx
@@ -1272,6 +1272,11 @@
           <t>Moon,</t>
         </is>
       </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>name|ab</t>
+        </is>
+      </c>
       <c r="O9" s="0" t="inlineStr">
         <is>
           <t>on</t>
@@ -2184,6 +2189,11 @@
           <t>Founders</t>
         </is>
       </c>
+      <c r="G20" s="0" t="inlineStr">
+        <is>
+          <t>gvscxdsv</t>
+        </is>
+      </c>
       <c r="I20" s="0" t="inlineStr">
         <is>
           <t>iron</t>
@@ -2197,6 +2207,11 @@
       <c r="P20" s="0" t="inlineStr">
         <is>
           <t>plate</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>riya|ft</t>
         </is>
       </c>
       <c r="S20" s="0" t="inlineStr">
@@ -2330,6 +2345,11 @@
           <t>b</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>ed|as</t>
+        </is>
+      </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
           <t>finding</t>
@@ -2362,7 +2382,7 @@
           <t>About</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="B24" s="0" t="inlineStr">
         <is>
           <t>bf</t>
         </is>
@@ -2625,7 +2645,7 @@
           <t>as</t>
         </is>
       </c>
-      <c r="S38" t="inlineStr">
+      <c r="S38" s="0" t="inlineStr">
         <is>
           <t>sdfgea</t>
         </is>

</xml_diff>

<commit_message>
added  the functionality of mic and copy file!!
</commit_message>
<xml_diff>
--- a/venv/words_library.xlsx
+++ b/venv/words_library.xlsx
@@ -1272,7 +1272,7 @@
           <t>Moon,</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="N9" s="0" t="inlineStr">
         <is>
           <t>name|ab</t>
         </is>
@@ -2209,7 +2209,7 @@
           <t>plate</t>
         </is>
       </c>
-      <c r="R20" t="inlineStr">
+      <c r="R20" s="0" t="inlineStr">
         <is>
           <t>riya|ft</t>
         </is>
@@ -2345,7 +2345,7 @@
           <t>b</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E23" s="0" t="inlineStr">
         <is>
           <t>ed|as</t>
         </is>

</xml_diff>